<commit_message>
added ops costs first draft
</commit_message>
<xml_diff>
--- a/TestCalc.xlsx
+++ b/TestCalc.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Servers</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Customer2</t>
+  </si>
+  <si>
+    <t>ops</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -416,18 +419,32 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <f>SUM(B2:B3)</f>
-        <v>150</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5">
+        <f>SUM(B2:B4)</f>
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
-        <f>SUM(E2:E3)</f>
-        <v>150</v>
+      <c r="E5">
+        <f>SUM(E2:E4)</f>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>